<commit_message>
update email technical & config prod
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Cybersourceocbcmdr/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Cybersourceocbcmdr/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Cybersourcevietin\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Cybersourceocbcmdr\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17227715-CA87-4BA3-A8A1-69CD211060B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D1716C-96CD-4BBB-BCF9-46C2F49276D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3852" yWindow="1536" windowWidth="17280" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>Captcha_RuleId</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -203,24 +200,6 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -240,6 +219,27 @@
   </si>
   <si>
     <t>RPA_Moon_Cred_Gmail</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_SheetIdConfig</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -666,10 +666,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -707,7 +707,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -2929,7 +2929,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2937,7 +2937,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2945,7 +2945,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2953,7 +2953,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
@@ -2961,7 +2961,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -2969,39 +2969,39 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>